<commit_message>
Evaluation updated n' values
</commit_message>
<xml_diff>
--- a/candidate-elimination-nprime/results.xlsx
+++ b/candidate-elimination-nprime/results.xlsx
@@ -4,10 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
-    <sheet name="17,6 - mismatch" sheetId="1" r:id="rId1"/>
+    <sheet name="9,2" sheetId="2" r:id="rId1"/>
+    <sheet name="11,3" sheetId="3" r:id="rId2"/>
+    <sheet name="13,4" sheetId="4" r:id="rId3"/>
+    <sheet name="15,5" sheetId="5" r:id="rId4"/>
+    <sheet name="17,6 - mismatch" sheetId="1" r:id="rId5"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="1">
   <si>
     <t>n'</t>
   </si>
@@ -70,17 +74,41 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -412,8 +440,747 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>5</v>
+      </c>
+      <c r="C1">
+        <v>6</v>
+      </c>
+      <c r="D1">
+        <v>7</v>
+      </c>
+      <c r="E1">
+        <v>8</v>
+      </c>
+      <c r="F1">
+        <v>9</v>
+      </c>
+      <c r="G1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>7.8E-2</v>
+      </c>
+      <c r="C2">
+        <v>6.2399999999999997E-2</v>
+      </c>
+      <c r="D2">
+        <v>4.6800000000000001E-2</v>
+      </c>
+      <c r="E2">
+        <v>4.6800000000000001E-2</v>
+      </c>
+      <c r="F2">
+        <v>4.6800000000000001E-2</v>
+      </c>
+      <c r="G2">
+        <v>3.1199999999999999E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>6.2399999999999997E-2</v>
+      </c>
+      <c r="C3">
+        <v>6.2399999999999997E-2</v>
+      </c>
+      <c r="D3">
+        <v>4.6800000000000001E-2</v>
+      </c>
+      <c r="E3">
+        <v>4.6800000000000001E-2</v>
+      </c>
+      <c r="F3">
+        <v>3.1199999999999999E-2</v>
+      </c>
+      <c r="G3">
+        <v>4.6800000000000001E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>7.8E-2</v>
+      </c>
+      <c r="C4">
+        <v>6.2399999999999997E-2</v>
+      </c>
+      <c r="D4">
+        <v>4.6800000000000001E-2</v>
+      </c>
+      <c r="E4">
+        <v>4.6800000000000001E-2</v>
+      </c>
+      <c r="F4">
+        <v>4.6800000000000001E-2</v>
+      </c>
+      <c r="G4">
+        <v>3.1199999999999999E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>7.8001000000000001E-2</v>
+      </c>
+      <c r="C5">
+        <v>6.2399999999999997E-2</v>
+      </c>
+      <c r="D5">
+        <v>4.6800000000000001E-2</v>
+      </c>
+      <c r="E5">
+        <v>4.6800000000000001E-2</v>
+      </c>
+      <c r="F5">
+        <v>3.1199999999999999E-2</v>
+      </c>
+      <c r="G5">
+        <v>4.6800000000000001E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>7.8001000000000001E-2</v>
+      </c>
+      <c r="C6">
+        <v>4.6800000000000001E-2</v>
+      </c>
+      <c r="D6">
+        <v>4.6800000000000001E-2</v>
+      </c>
+      <c r="E6">
+        <v>4.6800000000000001E-2</v>
+      </c>
+      <c r="F6">
+        <v>3.1199999999999999E-2</v>
+      </c>
+      <c r="G6">
+        <v>3.1199999999999999E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="B7">
+        <f>AVERAGE(B2:B6)</f>
+        <v>7.4880399999999986E-2</v>
+      </c>
+      <c r="C7">
+        <f t="shared" ref="C7:G7" si="0">AVERAGE(C2:C6)</f>
+        <v>5.9279999999999999E-2</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>4.6800000000000001E-2</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>4.6800000000000001E-2</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>3.7440000000000001E-2</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>3.7440000000000001E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>5</v>
+      </c>
+      <c r="C1">
+        <v>6</v>
+      </c>
+      <c r="D1">
+        <v>7</v>
+      </c>
+      <c r="E1">
+        <v>8</v>
+      </c>
+      <c r="F1">
+        <v>9</v>
+      </c>
+      <c r="G1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>0.42120099999999999</v>
+      </c>
+      <c r="C2">
+        <v>0.29640100000000003</v>
+      </c>
+      <c r="D2">
+        <v>0.20280000000000001</v>
+      </c>
+      <c r="E2">
+        <v>0.18720000000000001</v>
+      </c>
+      <c r="F2">
+        <v>0.140401</v>
+      </c>
+      <c r="G2">
+        <v>0.1404</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>0.42120099999999999</v>
+      </c>
+      <c r="C3">
+        <v>0.28079999999999999</v>
+      </c>
+      <c r="D3">
+        <v>0.20280100000000001</v>
+      </c>
+      <c r="E3">
+        <v>0.1716</v>
+      </c>
+      <c r="F3">
+        <v>0.156</v>
+      </c>
+      <c r="G3">
+        <v>0.124801</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>0.452401</v>
+      </c>
+      <c r="C4">
+        <v>0.3276</v>
+      </c>
+      <c r="D4">
+        <v>0.21840100000000001</v>
+      </c>
+      <c r="E4">
+        <v>0.18720000000000001</v>
+      </c>
+      <c r="F4">
+        <v>0.156</v>
+      </c>
+      <c r="G4">
+        <v>0.124801</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>0.42120000000000002</v>
+      </c>
+      <c r="C5">
+        <v>0.20280000000000001</v>
+      </c>
+      <c r="D5">
+        <v>0.18720000000000001</v>
+      </c>
+      <c r="E5">
+        <v>0.18720100000000001</v>
+      </c>
+      <c r="F5">
+        <v>0.1404</v>
+      </c>
+      <c r="G5">
+        <v>0.1404</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>0.40560099999999999</v>
+      </c>
+      <c r="C6">
+        <v>0.32760099999999998</v>
+      </c>
+      <c r="D6">
+        <v>0.21840000000000001</v>
+      </c>
+      <c r="E6">
+        <v>0.1716</v>
+      </c>
+      <c r="F6">
+        <v>0.140401</v>
+      </c>
+      <c r="G6">
+        <v>0.12479999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="B7">
+        <f>AVERAGE(B2:B6)</f>
+        <v>0.4243208</v>
+      </c>
+      <c r="C7">
+        <f t="shared" ref="C7:G7" si="0">AVERAGE(C2:C6)</f>
+        <v>0.28704040000000003</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>0.20592039999999998</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>0.18096019999999999</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>0.1466404</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>0.1310404</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G7"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>5</v>
+      </c>
+      <c r="C1">
+        <v>6</v>
+      </c>
+      <c r="D1">
+        <v>7</v>
+      </c>
+      <c r="E1">
+        <v>8</v>
+      </c>
+      <c r="F1">
+        <v>9</v>
+      </c>
+      <c r="G1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>2.2151999999999998</v>
+      </c>
+      <c r="C2">
+        <v>1.3104</v>
+      </c>
+      <c r="D2">
+        <v>0.96720200000000001</v>
+      </c>
+      <c r="E2">
+        <v>0.764401</v>
+      </c>
+      <c r="F2">
+        <v>0.68640199999999996</v>
+      </c>
+      <c r="G2">
+        <v>0.82680100000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2.5116100000000001</v>
+      </c>
+      <c r="C3">
+        <v>1.4663999999999999</v>
+      </c>
+      <c r="D3">
+        <v>1.1544000000000001</v>
+      </c>
+      <c r="E3">
+        <v>0.88920200000000005</v>
+      </c>
+      <c r="F3">
+        <v>1.0451999999999999</v>
+      </c>
+      <c r="G3">
+        <v>0.87360099999999996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>2.0903999999999998</v>
+      </c>
+      <c r="C4">
+        <v>1.248</v>
+      </c>
+      <c r="D4">
+        <v>0.904802</v>
+      </c>
+      <c r="E4">
+        <v>0.95160199999999995</v>
+      </c>
+      <c r="F4">
+        <v>0.67080099999999998</v>
+      </c>
+      <c r="G4">
+        <v>0.65520100000000003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>2.6988099999999999</v>
+      </c>
+      <c r="C5">
+        <v>1.7472000000000001</v>
+      </c>
+      <c r="D5">
+        <v>1.014</v>
+      </c>
+      <c r="E5">
+        <v>0.87360199999999999</v>
+      </c>
+      <c r="F5">
+        <v>0.68640100000000004</v>
+      </c>
+      <c r="G5">
+        <v>0.68640100000000004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>2.34</v>
+      </c>
+      <c r="C6">
+        <v>1.9188000000000001</v>
+      </c>
+      <c r="D6">
+        <v>1.014</v>
+      </c>
+      <c r="E6">
+        <v>0.73320200000000002</v>
+      </c>
+      <c r="F6">
+        <v>0.65520100000000003</v>
+      </c>
+      <c r="G6">
+        <v>0.74880100000000005</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="B7">
+        <f>AVERAGE(B2:B6)</f>
+        <v>2.3712040000000001</v>
+      </c>
+      <c r="C7">
+        <f t="shared" ref="C7:G7" si="0">AVERAGE(C2:C6)</f>
+        <v>1.53816</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>1.0108808000000002</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>0.84240179999999998</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>0.74880099999999994</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>0.75816099999999997</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>5</v>
+      </c>
+      <c r="C1">
+        <v>6</v>
+      </c>
+      <c r="D1">
+        <v>7</v>
+      </c>
+      <c r="E1">
+        <v>8</v>
+      </c>
+      <c r="F1">
+        <v>9</v>
+      </c>
+      <c r="G1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>17.737200000000001</v>
+      </c>
+      <c r="C2">
+        <v>12.792</v>
+      </c>
+      <c r="D2">
+        <v>10.8108</v>
+      </c>
+      <c r="E2">
+        <v>10.218</v>
+      </c>
+      <c r="F2">
+        <v>11.0136</v>
+      </c>
+      <c r="G2">
+        <v>11.8248</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>18.142800000000001</v>
+      </c>
+      <c r="C3">
+        <v>12.48</v>
+      </c>
+      <c r="D3">
+        <v>10.608000000000001</v>
+      </c>
+      <c r="E3">
+        <v>10.5456</v>
+      </c>
+      <c r="F3">
+        <v>11.107200000000001</v>
+      </c>
+      <c r="G3">
+        <v>11.778</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>17.940000000000001</v>
+      </c>
+      <c r="C4">
+        <v>12.6516</v>
+      </c>
+      <c r="D4">
+        <v>10.467599999999999</v>
+      </c>
+      <c r="E4">
+        <v>10.452</v>
+      </c>
+      <c r="F4">
+        <v>11.0916</v>
+      </c>
+      <c r="G4">
+        <v>12.074400000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>18.111599999999999</v>
+      </c>
+      <c r="C5">
+        <v>12.838800000000001</v>
+      </c>
+      <c r="D5">
+        <v>11.076000000000001</v>
+      </c>
+      <c r="E5">
+        <v>10.374000000000001</v>
+      </c>
+      <c r="F5">
+        <v>10.9512</v>
+      </c>
+      <c r="G5">
+        <v>11.871600000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>17.378399999999999</v>
+      </c>
+      <c r="C6">
+        <v>12.48</v>
+      </c>
+      <c r="D6">
+        <v>10.561199999999999</v>
+      </c>
+      <c r="E6">
+        <v>10.3116</v>
+      </c>
+      <c r="F6">
+        <v>10.904400000000001</v>
+      </c>
+      <c r="G6">
+        <v>11.9496</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="B7">
+        <f>AVERAGE(B2:B6)</f>
+        <v>17.862000000000002</v>
+      </c>
+      <c r="C7">
+        <f t="shared" ref="C7:G7" si="0">AVERAGE(C2:C6)</f>
+        <v>12.648480000000001</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>10.70472</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>10.380240000000001</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>11.0136</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>11.89968</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G7"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>